<commit_message>
[HomeView] Update image background
</commit_message>
<xml_diff>
--- a/documents/Others/TaskList.xlsx
+++ b/documents/Others/TaskList.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -288,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D272"/>
+  <dimension ref="A1:E272"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,9 +553,10 @@
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -559,15 +569,18 @@
       <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -577,8 +590,11 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -588,8 +604,11 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -599,8 +618,11 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -610,8 +632,11 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -621,8 +646,11 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -632,8 +660,11 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -643,8 +674,11 @@
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -654,8 +688,11 @@
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -665,8 +702,11 @@
       <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -676,15 +716,18 @@
       <c r="C12" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -694,16 +737,22 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -713,8 +762,11 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -724,8 +776,11 @@
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -735,8 +790,11 @@
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -746,8 +804,11 @@
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -757,8 +818,11 @@
       <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -768,18 +832,21 @@
       <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+      <c r="D21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="33" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="34" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="35" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1092,11 @@
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A13:XFD13"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D12 D14:D21">
+      <formula1>"Done,In Progress, Open"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1034,7 +1106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>